<commit_message>
created heat consumtpion and analysis function
</commit_message>
<xml_diff>
--- a/Current Building Characteristics.xlsx
+++ b/Current Building Characteristics.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\RenewEV-Heat-Loss-Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9569FCB-515B-488B-A53D-45BFD171980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F498C0-7DBC-4676-BE30-F48C260164AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F7AB01C9-9591-4175-8402-68F676A903F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="4" r:id="rId1"/>
     <sheet name="Elements" sheetId="2" r:id="rId2"/>
     <sheet name="Room Key" sheetId="1" r:id="rId3"/>
     <sheet name="Materials" sheetId="5" r:id="rId4"/>
-    <sheet name="Element Types" sheetId="3" r:id="rId5"/>
-    <sheet name="Effective Area" sheetId="7" r:id="rId6"/>
-    <sheet name="CO2 Conversion Factors" sheetId="6" r:id="rId7"/>
-    <sheet name="DHW" sheetId="8" r:id="rId8"/>
+    <sheet name="Effective Area" sheetId="7" r:id="rId5"/>
+    <sheet name="Dropdown" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="170">
   <si>
     <t>Element_Code</t>
   </si>
@@ -422,12 +420,6 @@
     <t>Roof/Wall Element</t>
   </si>
   <si>
-    <t>Scope 1 Emissions (kg CO2e/kWh)</t>
-  </si>
-  <si>
-    <t>UK Gov Jan 2022</t>
-  </si>
-  <si>
     <t>W4</t>
   </si>
   <si>
@@ -491,18 +483,6 @@
     <t>conductivity of soil under building (W/mK)</t>
   </si>
   <si>
-    <t>LPG</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
-    <t>Fuel (Gross CV)</t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
     <t>Mains Gas</t>
   </si>
   <si>
@@ -518,96 +498,15 @@
     <t>DHW source of heat</t>
   </si>
   <si>
-    <t>n_shower</t>
-  </si>
-  <si>
-    <t>n_wash</t>
-  </si>
-  <si>
-    <t>n_bath</t>
-  </si>
-  <si>
-    <t>n_sink</t>
-  </si>
-  <si>
     <t>2023-12-31  18:00:00</t>
   </si>
   <si>
     <t>2023-01-01  12:00:00</t>
   </si>
   <si>
-    <t>Number of showers in the house</t>
-  </si>
-  <si>
-    <t>Number of hand wash basins in the house</t>
-  </si>
-  <si>
-    <t>Number of baths</t>
-  </si>
-  <si>
-    <t>Number of kitchen sinks</t>
-  </si>
-  <si>
-    <t>hw_shower</t>
-  </si>
-  <si>
-    <t>Shower hot water load (L/unit)</t>
-  </si>
-  <si>
-    <t>hw_wash</t>
-  </si>
-  <si>
-    <t>Wash basin hot water load (L/unit)</t>
-  </si>
-  <si>
-    <t>hw_bath</t>
-  </si>
-  <si>
-    <t>Bath hot water load (L/unit)</t>
-  </si>
-  <si>
-    <t>hw_sink</t>
-  </si>
-  <si>
-    <t>Kitchen sink hot water load (L/unit)</t>
-  </si>
-  <si>
-    <t>t_reheat</t>
-  </si>
-  <si>
-    <t>reheat time (hours)</t>
-  </si>
-  <si>
-    <t>water_in</t>
-  </si>
-  <si>
-    <t>water inlet temperature (C)</t>
-  </si>
-  <si>
-    <t>water_out</t>
-  </si>
-  <si>
-    <t>water outlet temperature (C)</t>
-  </si>
-  <si>
-    <t>t_daily</t>
-  </si>
-  <si>
-    <t>daily heating time (hours)</t>
-  </si>
-  <si>
-    <t>t_active</t>
-  </si>
-  <si>
-    <t>active dhw days in the year (days/year)</t>
-  </si>
-  <si>
     <t>U-Value_Type</t>
   </si>
   <si>
-    <t>DG</t>
-  </si>
-  <si>
     <t>W1</t>
   </si>
   <si>
@@ -615,15 +514,48 @@
   </si>
   <si>
     <t>W3</t>
+  </si>
+  <si>
+    <t>fk</t>
+  </si>
+  <si>
+    <t>fRH</t>
+  </si>
+  <si>
+    <t>U-Value Type</t>
+  </si>
+  <si>
+    <t>Win - DG</t>
+  </si>
+  <si>
+    <t>Win - TG</t>
+  </si>
+  <si>
+    <t>Win - SinG</t>
+  </si>
+  <si>
+    <t>Win - SecG</t>
+  </si>
+  <si>
+    <t>D - Solid</t>
+  </si>
+  <si>
+    <t>D - DG</t>
+  </si>
+  <si>
+    <t>D - SinG</t>
+  </si>
+  <si>
+    <t>D- TG</t>
+  </si>
+  <si>
+    <t>D_Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00000"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -709,13 +641,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -726,6 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1043,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA64AD-AA06-4F69-BB92-B7A97995746A}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1246,8 +1175,8 @@
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="14" t="s">
-        <v>163</v>
+      <c r="B18" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="C18" t="s">
         <v>54</v>
@@ -1257,8 +1186,8 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>162</v>
+      <c r="B19" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>55</v>
@@ -1280,7 +1209,7 @@
         <v>107</v>
       </c>
       <c r="B21" s="2">
-        <f>SUM(Elements!P:P)</f>
+        <f>SUM(Elements!T:T)</f>
         <v>100</v>
       </c>
       <c r="C21" t="s">
@@ -1289,68 +1218,68 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B22" s="2">
         <v>1500</v>
       </c>
       <c r="C22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B23" s="2">
         <v>1900</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B24" s="2">
         <v>0.3</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" s="2">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1290,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1FF4F236-4E91-47E7-AD34-0B59BBD7B2D7}">
           <x14:formula1>
-            <xm:f>'CO2 Conversion Factors'!$A$2:$A$5</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>B26 B27</xm:sqref>
         </x14:dataValidation>
@@ -1373,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716C0F2C-B08A-4EA2-B90D-300B6914284F}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,16 +1314,19 @@
     <col min="2" max="2" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="9.90625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="10.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="19" max="23" width="7.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.26953125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="7.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.26953125" style="8" customWidth="1"/>
+    <col min="20" max="20" width="7.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="27" width="7.453125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1431,46 +1363,58 @@
       <c r="L1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="N1" s="7" t="s">
+      <c r="M1" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>95</v>
@@ -1502,46 +1446,56 @@
       <c r="L2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M2" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="N2" s="12">
-        <v>2</v>
+      <c r="M2" s="12">
+        <v>1</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="O2" s="12">
         <v>2</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>2</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T2" s="12">
         <v>0</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="U2" s="12">
         <v>90</v>
       </c>
-      <c r="R2" s="12">
+      <c r="V2" s="12">
         <v>0</v>
       </c>
-      <c r="S2" s="12">
+      <c r="W2" s="12">
         <v>1</v>
       </c>
-      <c r="T2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>138</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>93</v>
@@ -1573,46 +1527,56 @@
       <c r="L3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="N3" s="12">
+      <c r="M3" s="12">
+        <v>1</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="12">
         <v>1.5</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q3" s="12">
         <v>2</v>
       </c>
-      <c r="P3" s="12">
+      <c r="R3" s="12"/>
+      <c r="S3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T3" s="12">
         <v>0</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="U3" s="12">
         <v>90</v>
       </c>
-      <c r="R3" s="12">
+      <c r="V3" s="12">
         <v>-90</v>
       </c>
-      <c r="S3" s="12">
+      <c r="W3" s="12">
         <v>1</v>
       </c>
-      <c r="T3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>95</v>
@@ -1644,43 +1608,53 @@
       <c r="L4" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="N4" s="12">
-        <v>2</v>
+      <c r="M4" s="12">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="O4" s="12">
         <v>2</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>2</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4" s="12">
         <v>0</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="U4" s="12">
         <v>90</v>
       </c>
-      <c r="R4" s="12">
+      <c r="V4" s="12">
         <v>90</v>
       </c>
-      <c r="S4" s="12">
+      <c r="W4" s="12">
         <v>1</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="X4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>76</v>
@@ -1689,7 +1663,7 @@
         <v>93</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>94</v>
@@ -1715,43 +1689,53 @@
       <c r="L5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M5" s="12" t="s">
-        <v>94</v>
+      <c r="M5" s="12">
+        <v>1.4</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q5" s="12">
         <v>5</v>
       </c>
-      <c r="P5" s="12">
+      <c r="R5" s="12"/>
+      <c r="S5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T5" s="12">
         <v>0</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="U5" s="12">
         <v>90</v>
       </c>
-      <c r="R5" s="12">
+      <c r="V5" s="12">
         <v>180</v>
       </c>
-      <c r="S5" s="12">
+      <c r="W5" s="12">
         <v>1</v>
       </c>
-      <c r="T5" s="12">
+      <c r="X5" s="12">
         <v>1</v>
       </c>
-      <c r="U5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W5" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Y5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>76</v>
@@ -1760,7 +1744,7 @@
         <v>93</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>94</v>
@@ -1786,43 +1770,53 @@
       <c r="L6" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>94</v>
+      <c r="M6" s="12">
+        <v>1.4</v>
       </c>
       <c r="N6" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q6" s="12">
         <v>5</v>
       </c>
-      <c r="P6" s="12">
+      <c r="R6" s="12"/>
+      <c r="S6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T6" s="12">
         <v>0</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="U6" s="12">
         <v>90</v>
       </c>
-      <c r="R6" s="12">
+      <c r="V6" s="12">
         <v>0</v>
       </c>
-      <c r="S6" s="12">
+      <c r="W6" s="12">
         <v>1</v>
       </c>
-      <c r="T6" s="12">
+      <c r="X6" s="12">
         <v>1</v>
       </c>
-      <c r="U6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W6" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Y6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>76</v>
@@ -1831,7 +1825,7 @@
         <v>93</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>94</v>
@@ -1857,43 +1851,53 @@
       <c r="L7" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="12" t="s">
-        <v>94</v>
+      <c r="M7" s="12">
+        <v>1.4</v>
       </c>
       <c r="N7" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q7" s="12">
         <v>5</v>
       </c>
-      <c r="P7" s="12">
+      <c r="R7" s="12"/>
+      <c r="S7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T7" s="12">
         <v>0</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="U7" s="12">
         <v>90</v>
       </c>
-      <c r="R7" s="12">
+      <c r="V7" s="12">
         <v>90</v>
       </c>
-      <c r="S7" s="12">
+      <c r="W7" s="12">
         <v>1</v>
       </c>
-      <c r="T7" s="12">
+      <c r="X7" s="12">
         <v>1</v>
       </c>
-      <c r="U7" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Y7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>76</v>
@@ -1902,7 +1906,7 @@
         <v>93</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>94</v>
@@ -1928,43 +1932,53 @@
       <c r="L8" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="12" t="s">
-        <v>94</v>
+      <c r="M8" s="12">
+        <v>1.4</v>
       </c>
       <c r="N8" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q8" s="12">
         <v>5</v>
       </c>
-      <c r="P8" s="12">
+      <c r="R8" s="12"/>
+      <c r="S8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T8" s="12">
         <v>0</v>
       </c>
-      <c r="Q8" s="12">
+      <c r="U8" s="12">
         <v>90</v>
       </c>
-      <c r="R8" s="12">
+      <c r="V8" s="12">
         <v>-90</v>
       </c>
-      <c r="S8" s="12">
+      <c r="W8" s="12">
         <v>1</v>
       </c>
-      <c r="T8" s="12">
+      <c r="X8" s="12">
         <v>1</v>
       </c>
-      <c r="U8" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V8" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W8" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Y8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA8" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>69</v>
@@ -1973,7 +1987,7 @@
         <v>93</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>94</v>
@@ -1999,44 +2013,54 @@
       <c r="L9" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>94</v>
+      <c r="M9" s="12">
+        <v>1.26</v>
       </c>
       <c r="N9" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O9" s="12">
-        <f>10-O4</f>
+      <c r="O9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q9" s="12">
+        <f>10-Q4</f>
         <v>8</v>
       </c>
-      <c r="P9" s="12">
+      <c r="R9" s="12"/>
+      <c r="S9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="T9" s="12">
         <v>0</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="U9" s="12">
         <v>0</v>
       </c>
-      <c r="R9" s="12">
+      <c r="V9" s="12">
         <v>0</v>
       </c>
-      <c r="S9" s="12">
+      <c r="W9" s="12">
         <v>1</v>
       </c>
-      <c r="T9" s="12">
+      <c r="X9" s="12">
         <v>1</v>
       </c>
-      <c r="U9" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V9" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W9" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="Y9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA9" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>64</v>
@@ -2045,7 +2069,7 @@
         <v>93</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>94</v>
@@ -2071,37 +2095,47 @@
       <c r="L10" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="O10" s="12">
+      <c r="M10" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="N10" s="12">
+        <v>16</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q10" s="12">
         <v>10</v>
       </c>
-      <c r="P10" s="12">
-        <v>100</v>
-      </c>
-      <c r="Q10" s="12">
-        <v>0</v>
-      </c>
-      <c r="R10" s="12">
-        <v>0</v>
-      </c>
+      <c r="R10" s="12"/>
       <c r="S10" s="12">
         <v>1</v>
       </c>
       <c r="T10" s="12">
+        <v>100</v>
+      </c>
+      <c r="U10" s="12">
+        <v>0</v>
+      </c>
+      <c r="V10" s="12">
+        <v>0</v>
+      </c>
+      <c r="W10" s="12">
         <v>1</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="V10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="W10" s="12" t="s">
+      <c r="X10" s="12">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA10" s="12" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2109,10 +2143,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31461861-8C27-4353-B916-83BBEF5811A5}">
           <x14:formula1>
-            <xm:f>'Element Types'!$A$2:$A$56</xm:f>
+            <xm:f>Dropdown!$A$2:$A$56</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
@@ -2121,6 +2155,12 @@
             <xm:f>Materials!$A$2:$A$199</xm:f>
           </x14:formula1>
           <xm:sqref>E11:G1048576 E2:G2 C2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C18755C6-06E8-45AD-998D-5C7C44226C69}">
+          <x14:formula1>
+            <xm:f>Dropdown!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:P10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2265,7 +2305,7 @@
         <v>86</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>88</v>
@@ -2419,7 +2459,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" s="8">
         <v>130</v>
@@ -2480,10 +2520,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2495,150 +2535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13609CCC-BA72-4DF1-844A-507F100E80C1}">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>140</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE241666-7B8D-42CD-BC2E-BC0638B93994}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2659,23 +2560,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="19" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2716,7 +2617,7 @@
       <c r="L2" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="19"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -2747,237 +2648,167 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3EBB5D-1F3A-4DF3-88B7-5CADE8AC50FD}">
-  <dimension ref="A1:D5"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13609CCC-BA72-4DF1-844A-507F100E80C1}">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="13">
-        <v>0.21448999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="13">
-        <v>0.24676999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="13">
-        <v>0.21232999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="13">
-        <v>0.18315999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FF48CA-BE4C-4B22-9DA4-256F641563D7}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.6328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="2">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="2">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="2">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="2">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12" s="2">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" s="2">
-        <v>365</v>
-      </c>
-      <c r="C14" t="s">
-        <v>185</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2986,12 +2817,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005E6C8E2BBE97A449BF587258ABB90B5C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e50336969d1f6026fdc030928552f636">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da34839-94b1-4adb-9ce9-2bf1180dd981" xmlns:ns3="e21e7998-6f05-4771-9945-6b2b40d9b8dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="609895644b08c4e71b20ec11bc598037" ns2:_="" ns3:_="">
     <xsd:import namespace="9da34839-94b1-4adb-9ce9-2bf1180dd981"/>
@@ -3214,6 +3039,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3224,15 +3055,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA27988-4BDC-4DBB-93DD-2B86C53BCFE0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3251,6 +3073,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86AA0889-6486-4C22-A950-9F61B4B8A696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFAA5CEA-80BB-497C-B05C-1589868B6D5D}">
   <ds:schemaRefs>

</xml_diff>